<commit_message>
redesign sso support AD
</commit_message>
<xml_diff>
--- a/ldap_config_files/ldap_config_v0.1.xlsx
+++ b/ldap_config_files/ldap_config_v0.1.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>name</t>
   </si>
@@ -47,9 +47,6 @@
     <t>method</t>
   </si>
   <si>
-    <t>licensee_id</t>
-  </si>
-  <si>
     <t>account_password</t>
   </si>
   <si>
@@ -90,6 +87,21 @@
   </si>
   <si>
     <t>dc=dctest, dc=local</t>
+  </si>
+  <si>
+    <t>ldap.admin@dctest.local</t>
+  </si>
+  <si>
+    <t>Cc123456</t>
+  </si>
+  <si>
+    <t>domain</t>
+  </si>
+  <si>
+    <t>mo.laxino.com</t>
+  </si>
+  <si>
+    <t>dctest.local</t>
   </si>
 </sst>
 </file>
@@ -450,7 +462,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
@@ -464,14 +478,14 @@
     <col min="8" max="8" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23" style="1" customWidth="1"/>
     <col min="12" max="12" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -486,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>4</v>
@@ -498,36 +512,36 @@
         <v>6</v>
       </c>
       <c r="J1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
-        <v>1000</v>
+      <c r="A2" s="2" t="s">
+        <v>24</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="D2" s="2">
         <v>3268</v>
       </c>
       <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
@@ -536,32 +550,36 @@
       <c r="L2" s="2"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
-        <v>20000</v>
+      <c r="A3" s="2" t="s">
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="2">
         <v>3268</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+      <c r="K3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>